<commit_message>
changed pro mini link and price
</commit_message>
<xml_diff>
--- a/Electronics/MCU_details_and_scoring.xlsx
+++ b/Electronics/MCU_details_and_scoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kjans\AppData\Local\Packages\CanonicalGroupLimited.UbuntuonWindows_79rhkp1fndgsc\LocalState\rootfs\home\kj123\BME590-LightDHF\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8FB169-07DB-4CB8-9E2D-6C58C502DBF8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828378D2-FB10-4AB5-8135-AB56D5A5C5E2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8424" xr2:uid="{7E3EB27C-7943-4593-978D-AB1FE681741A}"/>
   </bookViews>
@@ -187,7 +187,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -196,6 +196,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -515,7 +516,7 @@
   <dimension ref="A2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,9 +582,8 @@
       <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="6" t="str">
-        <f>"$" &amp;ROUND(9.99/3,2) &amp; " per piece"</f>
-        <v>$3.33 per piece</v>
+      <c r="E4" s="8">
+        <v>12.99</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>6</v>

</xml_diff>